<commit_message>
Final updates and cleaning
</commit_message>
<xml_diff>
--- a/DIFFIT.xlsx
+++ b/DIFFIT.xlsx
@@ -614,7 +614,7 @@
         <v>2.551761356829118</v>
       </c>
       <c r="G7" t="n">
-        <v>1.068054589959113</v>
+        <v>1.068054589959119</v>
       </c>
     </row>
     <row r="8">
@@ -631,13 +631,13 @@
         <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>71.71412517321424</v>
+        <v>71.71412517321423</v>
       </c>
       <c r="F8" t="n">
-        <v>2.389167539579418</v>
+        <v>2.389167539579404</v>
       </c>
       <c r="G8" t="n">
-        <v>1.186461189122596</v>
+        <v>1.18646118912258</v>
       </c>
     </row>
     <row r="9">
@@ -654,10 +654,10 @@
         <v>4</v>
       </c>
       <c r="E9" t="n">
-        <v>73.22539713601785</v>
+        <v>73.22539713601786</v>
       </c>
       <c r="F9" t="n">
-        <v>1.511271962803605</v>
+        <v>1.511271962803633</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -679,10 +679,10 @@
         <v>4</v>
       </c>
       <c r="E10" t="n">
-        <v>74.96442182579653</v>
+        <v>74.96442182579652</v>
       </c>
       <c r="F10" t="n">
-        <v>1.739024689778688</v>
+        <v>1.73902468977866</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -707,10 +707,10 @@
         <v>76.97811393935504</v>
       </c>
       <c r="F11" t="n">
-        <v>2.013692113558506</v>
+        <v>2.01369211355852</v>
       </c>
       <c r="G11" t="n">
-        <v>1.105533946703554</v>
+        <v>1.105533946703562</v>
       </c>
     </row>
     <row r="12">
@@ -1157,7 +1157,7 @@
         <v>0.3688546176090313</v>
       </c>
       <c r="G30" t="n">
-        <v>1.182270586775136</v>
+        <v>1.18227058677519</v>
       </c>
     </row>
     <row r="31">
@@ -1199,10 +1199,10 @@
         <v>12</v>
       </c>
       <c r="E32" t="n">
-        <v>97.43830579432425</v>
+        <v>97.43830579432426</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3070834766977271</v>
+        <v>0.3070834766977413</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1227,10 +1227,10 @@
         <v>97.75029411724714</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3119883229228861</v>
+        <v>0.3119883229228719</v>
       </c>
       <c r="G33" t="n">
-        <v>1.118854373316714</v>
+        <v>1.118854373316663</v>
       </c>
     </row>
     <row r="34">
@@ -3447,7 +3447,7 @@
         <v>6.989033550768639</v>
       </c>
       <c r="G4" t="n">
-        <v>1.326214285217869</v>
+        <v>1.32621428521787</v>
       </c>
     </row>
     <row r="5">
@@ -3464,13 +3464,13 @@
         <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>57.06785588639932</v>
+        <v>57.06785588639931</v>
       </c>
       <c r="F5" t="n">
-        <v>5.269912734819087</v>
+        <v>5.26991273481908</v>
       </c>
       <c r="G5" t="n">
-        <v>1.410179550711695</v>
+        <v>1.410179550711693</v>
       </c>
     </row>
     <row r="6">
@@ -3490,7 +3490,7 @@
         <v>59.32809199926973</v>
       </c>
       <c r="F6" t="n">
-        <v>2.260236112870409</v>
+        <v>2.260236112870416</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3685,7 +3685,7 @@
         <v>1.700954377839921</v>
       </c>
       <c r="G14" t="n">
-        <v>1.076944392115435</v>
+        <v>1.076944392115426</v>
       </c>
     </row>
     <row r="15">
@@ -3727,13 +3727,13 @@
         <v>6</v>
       </c>
       <c r="E16" t="n">
-        <v>83.3427618104286</v>
+        <v>83.34276181042861</v>
       </c>
       <c r="F16" t="n">
-        <v>1.579426375486989</v>
+        <v>1.579426375487003</v>
       </c>
       <c r="G16" t="n">
-        <v>1.010394177874695</v>
+        <v>1.010394177874713</v>
       </c>
     </row>
     <row r="17">
@@ -3753,10 +3753,10 @@
         <v>84.90594023135856</v>
       </c>
       <c r="F17" t="n">
-        <v>1.563178420929958</v>
+        <v>1.563178420929944</v>
       </c>
       <c r="G17" t="n">
-        <v>1.253729016297797</v>
+        <v>1.253729016297786</v>
       </c>
     </row>
     <row r="18">
@@ -6404,7 +6404,7 @@
         <v>2.927368745190137</v>
       </c>
       <c r="G6" t="n">
-        <v>1.031830792823895</v>
+        <v>1.0318307928239</v>
       </c>
     </row>
     <row r="7">
@@ -6421,13 +6421,13 @@
         <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>76.83068722613498</v>
+        <v>76.83068722613497</v>
       </c>
       <c r="F7" t="n">
-        <v>2.837062787376766</v>
+        <v>2.837062787376752</v>
       </c>
       <c r="G7" t="n">
-        <v>1.617402563256685</v>
+        <v>1.617402563256664</v>
       </c>
     </row>
     <row r="8">
@@ -6447,7 +6447,7 @@
         <v>78.3837523926244</v>
       </c>
       <c r="F8" t="n">
-        <v>1.553065166489418</v>
+        <v>1.553065166489432</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -6519,10 +6519,10 @@
         <v>5</v>
       </c>
       <c r="E11" t="n">
-        <v>83.43783980775753</v>
+        <v>83.43783980775751</v>
       </c>
       <c r="F11" t="n">
-        <v>1.65269787688193</v>
+        <v>1.652697876881916</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -6547,10 +6547,10 @@
         <v>85.19192555723492</v>
       </c>
       <c r="F12" t="n">
-        <v>1.754085749477397</v>
+        <v>1.754085749477412</v>
       </c>
       <c r="G12" t="n">
-        <v>1.094563112043066</v>
+        <v>1.094563112043065</v>
       </c>
     </row>
     <row r="13">
@@ -6567,10 +6567,10 @@
         <v>5</v>
       </c>
       <c r="E13" t="n">
-        <v>86.18486447909083</v>
+        <v>86.18486447909082</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9929389218559095</v>
+        <v>0.9929389218558953</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -6595,10 +6595,10 @@
         <v>87.78740866332092</v>
       </c>
       <c r="F14" t="n">
-        <v>1.602544184230084</v>
+        <v>1.602544184230098</v>
       </c>
       <c r="G14" t="n">
-        <v>1.347033053908984</v>
+        <v>1.347033053908996</v>
       </c>
     </row>
     <row r="15">
@@ -6621,7 +6621,7 @@
         <v>1.189684380483186</v>
       </c>
       <c r="G15" t="n">
-        <v>1.135299089295309</v>
+        <v>1.135299089295293</v>
       </c>
     </row>
     <row r="16">
@@ -6638,13 +6638,13 @@
         <v>6</v>
       </c>
       <c r="E16" t="n">
-        <v>90.02499697652163</v>
+        <v>90.02499697652165</v>
       </c>
       <c r="F16" t="n">
-        <v>1.047903932717531</v>
+        <v>1.047903932717546</v>
       </c>
       <c r="G16" t="n">
-        <v>1.303861462882254</v>
+        <v>1.303861462882294</v>
       </c>
     </row>
     <row r="17">
@@ -6664,10 +6664,10 @@
         <v>90.82868967129696</v>
       </c>
       <c r="F17" t="n">
-        <v>0.8036926947753216</v>
+        <v>0.8036926947753074</v>
       </c>
       <c r="G17" t="n">
-        <v>1.083126199669359</v>
+        <v>1.08312619966934</v>
       </c>
     </row>
     <row r="18">
@@ -10921,7 +10921,7 @@
         <v>0.0155961717434252</v>
       </c>
       <c r="G68" t="n">
-        <v>1.096679992349715</v>
+        <v>1.096679992348619</v>
       </c>
     </row>
     <row r="69">
@@ -10938,13 +10938,13 @@
         <v>6</v>
       </c>
       <c r="E69" t="n">
-        <v>99.86762795083375</v>
+        <v>99.86762795083376</v>
       </c>
       <c r="F69" t="n">
-        <v>0.01422126039703642</v>
+        <v>0.01422126039705063</v>
       </c>
       <c r="G69" t="n">
-        <v>1.038395258887526</v>
+        <v>1.038395258889641</v>
       </c>
     </row>
     <row r="70">
@@ -10964,10 +10964,10 @@
         <v>99.88132337198992</v>
       </c>
       <c r="F70" t="n">
-        <v>0.01369542115617151</v>
+        <v>0.01369542115615729</v>
       </c>
       <c r="G70" t="n">
-        <v>1.002852674801187</v>
+        <v>1.002852674800147</v>
       </c>
     </row>
     <row r="71">
@@ -12978,10 +12978,10 @@
         <v>5</v>
       </c>
       <c r="E17" t="n">
-        <v>75.91925366732896</v>
+        <v>75.91925366732895</v>
       </c>
       <c r="F17" t="n">
-        <v>0.4822872290788069</v>
+        <v>0.4822872290787927</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -13003,7 +13003,7 @@
         <v>5</v>
       </c>
       <c r="E18" t="n">
-        <v>76.48695719973701</v>
+        <v>76.48695719973699</v>
       </c>
       <c r="F18" t="n">
         <v>0.5677035324080464</v>
@@ -13031,7 +13031,7 @@
         <v>77.01966679564535</v>
       </c>
       <c r="F19" t="n">
-        <v>0.5327095959083437</v>
+        <v>0.5327095959083579</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -13253,10 +13253,10 @@
         <v>7</v>
       </c>
       <c r="E28" t="n">
-        <v>82.11149050948178</v>
+        <v>82.1114905094818</v>
       </c>
       <c r="F28" t="n">
-        <v>0.5851385493191401</v>
+        <v>0.5851385493191543</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -13281,7 +13281,7 @@
         <v>82.69828968637687</v>
       </c>
       <c r="F29" t="n">
-        <v>0.5867991768950844</v>
+        <v>0.5867991768950702</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -17005,7 +17005,7 @@
         <v>0.1703455402465579</v>
       </c>
       <c r="G67" t="n">
-        <v>1.062952316962269</v>
+        <v>1.062952316962363</v>
       </c>
     </row>
     <row r="68">
@@ -17022,13 +17022,13 @@
         <v>10</v>
       </c>
       <c r="E68" t="n">
-        <v>97.84026830343197</v>
+        <v>97.84026830343196</v>
       </c>
       <c r="F68" t="n">
-        <v>0.1602569913327585</v>
+        <v>0.1602569913327443</v>
       </c>
       <c r="G68" t="n">
-        <v>1.063065467208857</v>
+        <v>1.063065467208662</v>
       </c>
     </row>
     <row r="69">
@@ -17048,10 +17048,10 @@
         <v>97.99101818316753</v>
       </c>
       <c r="F69" t="n">
-        <v>0.1507498797355566</v>
+        <v>0.1507498797355709</v>
       </c>
       <c r="G69" t="n">
-        <v>1.080254451777597</v>
+        <v>1.080254451777699</v>
       </c>
     </row>
     <row r="70">

</xml_diff>